<commit_message>
Add new Sensor Class
</commit_message>
<xml_diff>
--- a/Pinout_ESP8266.xlsx
+++ b/Pinout_ESP8266.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Todo" sheetId="3" r:id="rId1"/>
+    <sheet name="Pinout ESP" sheetId="1" r:id="rId2"/>
+    <sheet name="Temp Sensors" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Blue</t>
   </si>
@@ -47,6 +47,129 @@
   <si>
     <t>First is as Output (8 mechanic relais and 8 solid state relais)
 Second as Input for current state of heating outputs</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>CS (Chip select) Ethernet</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SCL MCP23017</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>SDA MCP23017</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Int Port 1 MCP23017</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Int Port 2 MCP23017</t>
+  </si>
+  <si>
+    <t>GPIO16</t>
+  </si>
+  <si>
+    <t>GPIO5</t>
+  </si>
+  <si>
+    <t>GPIO4</t>
+  </si>
+  <si>
+    <t>GPIO0</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>GPIO14</t>
+  </si>
+  <si>
+    <t>GPIO12</t>
+  </si>
+  <si>
+    <t>GPIO13</t>
+  </si>
+  <si>
+    <t>GPIO15</t>
+  </si>
+  <si>
+    <t>SCLK Ethernet</t>
+  </si>
+  <si>
+    <t>MISO Ethernet</t>
+  </si>
+  <si>
+    <t>MOSI Ethernet</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>Serial Interface</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>GPIO1</t>
+  </si>
+  <si>
+    <t>ADC0</t>
+  </si>
+  <si>
+    <t>Measurement Gas quality of ventilation</t>
+  </si>
+  <si>
+    <t>switch Power for Gas sensor (CS not for INPUT it could get problems)</t>
+  </si>
+  <si>
+    <t>Air con - incoming air - in</t>
+  </si>
+  <si>
+    <t>Air con - incoming air - out</t>
+  </si>
+  <si>
+    <t>Air con - outcomig air - in</t>
+  </si>
+  <si>
+    <t>Air con - outcomig air - out</t>
+  </si>
+  <si>
+    <t>Heat pump -  heat exchanger</t>
+  </si>
+  <si>
+    <t>Solar - heat exchanger</t>
+  </si>
+  <si>
+    <t>Earth heat - optional</t>
   </si>
 </sst>
 </file>
@@ -105,16 +228,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>315411</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>639261</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>124546</xdr:rowOff>
+      <xdr:rowOff>19771</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -131,7 +254,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="352425" y="1438275"/>
+          <a:off x="5724525" y="1333500"/>
           <a:ext cx="7783011" cy="5163271"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -431,67 +554,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -499,14 +564,247 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add struct für output & sensors
</commit_message>
<xml_diff>
--- a/Pinout_ESP8266.xlsx
+++ b/Pinout_ESP8266.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Blue</t>
   </si>
@@ -170,15 +170,58 @@
   </si>
   <si>
     <t>Earth heat - optional</t>
+  </si>
+  <si>
+    <t>HTML side for name mapping Sensors</t>
+  </si>
+  <si>
+    <t>HTML side for name mapping digital inputs</t>
+  </si>
+  <si>
+    <t>HTML side for name mapping digital outputs</t>
+  </si>
+  <si>
+    <t>MQTT active</t>
+  </si>
+  <si>
+    <t>current state of Output (on/off/auto)</t>
+  </si>
+  <si>
+    <t>Output name</t>
+  </si>
+  <si>
+    <t>current state of Input (on/off)</t>
+  </si>
+  <si>
+    <t>Input name</t>
+  </si>
+  <si>
+    <t>Equal to Input</t>
+  </si>
+  <si>
+    <t>current state of Sensor (Value in °C)</t>
+  </si>
+  <si>
+    <t>Sensor name</t>
+  </si>
+  <si>
+    <t>Sensor address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,11 +248,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -554,13 +598,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Gave the program a better structure
</commit_message>
<xml_diff>
--- a/Pinout_ESP8266.xlsx
+++ b/Pinout_ESP8266.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Blue</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Sensor address</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Add Datalog for restart ESP</t>
   </si>
 </sst>
 </file>
@@ -598,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E9"/>
+  <dimension ref="A3:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,64 +617,108 @@
     <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" t="s">
         <v>53</v>
       </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
       <c r="E3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
       <c r="C4" t="s">
         <v>54</v>
       </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
       <c r="E4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
       <c r="C5" t="s">
         <v>55</v>
       </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
       <c r="E5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
       <c r="C6" t="s">
         <v>56</v>
       </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
       <c r="E6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
       <c r="C7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>